<commit_message>
Fix für Dateiname ' auf alle Daten ausgerollt
</commit_message>
<xml_diff>
--- a/wortliste/redewendungen.xlsx
+++ b/wortliste/redewendungen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pixel\Documents\Repos\tmp\hillerplatt.de\wortliste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA50167-B602-43CF-A942-8F0248642D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A8631D-22B6-47FB-A715-64D15ADE28CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6862AAEA-ED9A-42B0-8BFD-4A1D1A3BF1D7}"/>
   </bookViews>
@@ -50,9 +50,6 @@
     <t>Ein Hund auf dem Hof hat es besser als ….</t>
   </si>
   <si>
-    <t>Leiber'n Spatz inne Hand, wie ne Diuben uppen Doake.</t>
-  </si>
-  <si>
     <t>Lieber einen Spatz in der Hand, als eine Taube auf dem Dach.</t>
   </si>
   <si>
@@ -134,9 +131,6 @@
     <t>Er hat so viel Glück, dass ihm alles gelingt.</t>
   </si>
   <si>
-    <t>Für'n Sack vull Geld nimmp de Welt den Heot af.</t>
-  </si>
-  <si>
     <t>Geld regiert die Welt.</t>
   </si>
   <si>
@@ -170,9 +164,6 @@
     <t>Dem ist wohl eine Laus über die Leber gelaufen.</t>
   </si>
   <si>
-    <t>De kieket sick nich moal mit'm Oarse an.</t>
-  </si>
-  <si>
     <t>Die sind ganz und gar zerstritten.</t>
   </si>
   <si>
@@ -182,15 +173,9 @@
     <t>Er ist stolz.</t>
   </si>
   <si>
-    <t>Et was man nur sau'n Dopp.</t>
-  </si>
-  <si>
     <t>Es war nur so ein kleines Stück.</t>
   </si>
   <si>
-    <t>Dat Schwien noa'n Bärn bringen.</t>
-  </si>
-  <si>
     <t>Das Schwein vom Eber decken lassen.</t>
   </si>
   <si>
@@ -204,9 +189,6 @@
   </si>
   <si>
     <t xml:space="preserve">Guter Ertrag bei der Getreideernte. </t>
-  </si>
-  <si>
-    <t>Hiller Begriff für  "auf dem Friedhof liegen".</t>
   </si>
   <si>
     <t>Hei socket dorhenn.</t>
@@ -234,9 +216,6 @@
 Antwort: Du hast noch gar keinen Rücken. </t>
   </si>
   <si>
-    <t>Wi wütt 'n Hitken fillen.</t>
-  </si>
-  <si>
     <t>Wir wollen zum Vergnügen ausgehen.</t>
   </si>
   <si>
@@ -288,9 +267,6 @@
     <t>Ich bin doch nicht dein Laufbursche.</t>
   </si>
   <si>
-    <t>Hei weol mi an't Lear.</t>
-  </si>
-  <si>
     <t>Er wollte mir ans Leder.</t>
   </si>
   <si>
@@ -348,9 +324,6 @@
     <t>Hast du deine Siebensachen gepackt?</t>
   </si>
   <si>
-    <t>Et was öhne an'n Pierk togen.</t>
-  </si>
-  <si>
     <t>Es ist ihm sehr nahe gegangen.</t>
   </si>
   <si>
@@ -381,9 +354,6 @@
     <t>Heftiger, teils unberechtigter Kritik ausgesetzt sein.</t>
   </si>
   <si>
-    <t>Van'n Beinen dat räaßet.</t>
-  </si>
-  <si>
     <t>Ausruhen nach anstrengender, körperlicher Tätigkeit.</t>
   </si>
   <si>
@@ -393,9 +363,6 @@
     <t>Halt deinen Mund!</t>
   </si>
   <si>
-    <t>An geden Schliepstein es'n Draaiher.</t>
-  </si>
-  <si>
     <t>Es gibt für alles eine Lösung.</t>
   </si>
   <si>
@@ -571,9 +538,6 @@
   </si>
   <si>
     <t>Darauf kannst du dich verlassen.</t>
-  </si>
-  <si>
-    <t>Up'n Pinn trehen.</t>
   </si>
   <si>
     <t>Gas geben, sich beeilen</t>
@@ -736,9 +700,6 @@
     <t>Taubenzucht und Imkerei sind kostspielige Hobbys.</t>
   </si>
   <si>
-    <t>Wi oarbert'e bian.</t>
-  </si>
-  <si>
     <t>Wir arbeiten ohne Druck weiter.</t>
   </si>
   <si>
@@ -770,9 +731,6 @@
   </si>
   <si>
     <t>Schall eck di eine langen︖</t>
-  </si>
-  <si>
-    <t>Hei flötket iut'n lesten Looke.</t>
   </si>
   <si>
     <t>Hei häff Nuck up einen.</t>
@@ -817,6 +775,48 @@
   </si>
   <si>
     <t>De gloaihet wi en Leggeheohn.</t>
+  </si>
+  <si>
+    <t>Leiber’n Spatz inne Hand, wie ne Diuben uppen Doake.</t>
+  </si>
+  <si>
+    <t>Für’n Sack vull Geld nimmp de Welt den Heot af.</t>
+  </si>
+  <si>
+    <t>De kieket sick nich moal mit’m Oarse an.</t>
+  </si>
+  <si>
+    <t>Et was man nur sau’n Dopp.</t>
+  </si>
+  <si>
+    <t>Dat Schwien noa’n Bärn bringen.</t>
+  </si>
+  <si>
+    <t>Wi wütt ’n Hitken fillen.</t>
+  </si>
+  <si>
+    <t>Hei weol mi an’t Lear.</t>
+  </si>
+  <si>
+    <t>Hei flötket iut’n lesten Looke.</t>
+  </si>
+  <si>
+    <t>Et was öhne an’n Pierk togen.</t>
+  </si>
+  <si>
+    <t>Van’n Beinen dat räaßet.</t>
+  </si>
+  <si>
+    <t>An geden Schliepstein es’n Draaiher.</t>
+  </si>
+  <si>
+    <t>Up’n Pinn trehen.</t>
+  </si>
+  <si>
+    <t>Wi oarbert’e bian.</t>
+  </si>
+  <si>
+    <t>Hiller Begriff für "auf dem Friedhof liegen".</t>
   </si>
 </sst>
 </file>
@@ -1252,8 +1252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE573C9-6D8B-4805-BB18-E43F1EE05309}">
   <dimension ref="A1:B130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="H88" sqref="H88"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1264,10 +1264,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -1288,1018 +1288,1018 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>32</v>
+        <v>246</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>44</v>
+        <v>247</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>48</v>
+        <v>248</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>50</v>
+        <v>249</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>56</v>
+        <v>258</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>65</v>
+        <v>250</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>32</v>
+        <v>246</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>83</v>
+        <v>251</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>103</v>
+        <v>253</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>114</v>
+        <v>254</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>118</v>
+        <v>255</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>178</v>
+        <v>256</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A100" s="8" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>232</v>
+        <v>257</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Falsch übersetzte Redewendung "auf der Kippe stehen" entfernt.
</commit_message>
<xml_diff>
--- a/wortliste/redewendungen.xlsx
+++ b/wortliste/redewendungen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pixel\Documents\Repos\tmp\hillerplatt.de\wortliste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A8631D-22B6-47FB-A715-64D15ADE28CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21CA1ED1-B3D9-4747-AEBB-51EA2EFCC0B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6862AAEA-ED9A-42B0-8BFD-4A1D1A3BF1D7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{6862AAEA-ED9A-42B0-8BFD-4A1D1A3BF1D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="258">
   <si>
     <t>Et es en Klärd körler wurn.</t>
   </si>
@@ -241,9 +241,6 @@
   </si>
   <si>
     <t>Jemanden zur Verantwortung ziehen.</t>
-  </si>
-  <si>
-    <t>Auf der Kippe stehen.</t>
   </si>
   <si>
     <t>Wenn de Ziergen Woater süht, denn well se lappen.</t>
@@ -1250,10 +1247,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE573C9-6D8B-4805-BB18-E43F1EE05309}">
-  <dimension ref="A1:B130"/>
+  <dimension ref="A1:B129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:XFD41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1264,10 +1261,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>239</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -1288,7 +1285,7 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -1400,7 +1397,7 @@
     </row>
     <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>31</v>
@@ -1448,7 +1445,7 @@
     </row>
     <row r="24" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>42</v>
@@ -1464,7 +1461,7 @@
     </row>
     <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>45</v>
@@ -1472,7 +1469,7 @@
     </row>
     <row r="27" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>46</v>
@@ -1496,10 +1493,10 @@
     </row>
     <row r="30" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -1512,7 +1509,7 @@
     </row>
     <row r="32" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>53</v>
@@ -1536,7 +1533,7 @@
     </row>
     <row r="35" spans="1:2" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>58</v>
@@ -1544,7 +1541,7 @@
     </row>
     <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>59</v>
@@ -1584,15 +1581,15 @@
     </row>
     <row r="41" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>246</v>
+        <v>68</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>69</v>
+        <v>229</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>70</v>
@@ -1600,25 +1597,25 @@
     </row>
     <row r="43" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>230</v>
+        <v>71</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B45" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1626,85 +1623,85 @@
       <c r="A46" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>252</v>
+        <v>77</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B50" s="1" t="s">
+      <c r="A50" s="5" t="s">
         <v>83</v>
       </c>
+      <c r="B50" s="5" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="51" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B51" s="5" t="s">
+      <c r="A51" s="1" t="s">
         <v>85</v>
       </c>
+      <c r="B51" s="1" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="52" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B52" s="1" t="s">
+      <c r="A52" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>243</v>
+      <c r="B53" s="5" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>92</v>
+        <v>231</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>93</v>
@@ -1712,7 +1709,7 @@
     </row>
     <row r="57" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>232</v>
+        <v>252</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>94</v>
@@ -1720,47 +1717,47 @@
     </row>
     <row r="58" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>253</v>
+        <v>95</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B61" s="5" t="s">
+      <c r="A61" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="B62" s="1" t="s">
+      <c r="A62" s="5" t="s">
         <v>102</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>103</v>
+        <v>253</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>104</v>
@@ -1768,15 +1765,15 @@
     </row>
     <row r="64" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>254</v>
+        <v>105</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>106</v>
+        <v>254</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>107</v>
@@ -1784,23 +1781,23 @@
     </row>
     <row r="66" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>255</v>
+        <v>108</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="5" t="s">
-        <v>109</v>
+      <c r="A67" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>111</v>
+      <c r="A68" s="5" t="s">
+        <v>232</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>112</v>
@@ -1808,207 +1805,207 @@
     </row>
     <row r="69" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>233</v>
+        <v>113</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B76" s="5" t="s">
+      <c r="A76" s="1" t="s">
         <v>127</v>
       </c>
+      <c r="B76" s="1" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="77" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B77" s="1" t="s">
+      <c r="A77" s="5" t="s">
         <v>129</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A87" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="B87" s="5" t="s">
+    </row>
+    <row r="87" spans="1:2" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="A87" s="6" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="A88" s="6" t="s">
+      <c r="B87" s="7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="B88" s="7" t="s">
-        <v>238</v>
+      <c r="B88" s="5" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>161</v>
+        <v>243</v>
       </c>
       <c r="B94" s="5" t="s">
         <v>162</v>
@@ -2016,7 +2013,7 @@
     </row>
     <row r="95" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="B95" s="5" t="s">
         <v>163</v>
@@ -2024,191 +2021,191 @@
     </row>
     <row r="96" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A98" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="A99" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="B96" s="5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A97" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A99" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="B99" s="5" t="s">
+      <c r="B99" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="A100" s="8" t="s">
-        <v>235</v>
-      </c>
       <c r="B100" s="2" t="s">
-        <v>241</v>
+        <v>170</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B111" s="2" t="s">
+      <c r="A111" s="1" t="s">
         <v>191</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="B114" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B114" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>236</v>
+        <v>198</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>205</v>
+        <v>236</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>206</v>
@@ -2216,55 +2213,55 @@
     </row>
     <row r="120" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>237</v>
+        <v>207</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>218</v>
+        <v>256</v>
       </c>
       <c r="B126" s="2" t="s">
         <v>219</v>
@@ -2272,34 +2269,26 @@
     </row>
     <row r="127" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>257</v>
+        <v>220</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A130" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>